<commit_message>
Major improvement to the handling of styles. Drops IXLFill.PatternBackgroundColor!
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Columns/ColumnCollection.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Columns/ColumnCollection.xlsx
@@ -42,43 +42,36 @@
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF696969"/>
-        <x:bgColor rgb="FF696969"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FFFF0000"/>
-        <x:bgColor rgb="FFFF0000"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF0000FF"/>
-        <x:bgColor rgb="FF0000FF"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FFFF1493"/>
-        <x:bgColor rgb="FFFF1493"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FFFFA500"/>
-        <x:bgColor rgb="FFFFA500"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF40E0D0"/>
-        <x:bgColor rgb="FF40E0D0"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF00FFFF"/>
-        <x:bgColor rgb="FF00FFFF"/>
       </x:patternFill>
     </x:fill>
   </x:fills>

</xml_diff>

<commit_message>
Save calculated column formula in table field (#528)
* Save calculated column formula in table field

* Add data format id to table columns if data format is consistent.

* Major improvement to the handling of styles. Drops IXLFill.PatternBackgroundColor!

* Remove property changed vars on XLFill
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Columns/ColumnCollection.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Columns/ColumnCollection.xlsx
@@ -42,43 +42,36 @@
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF696969"/>
-        <x:bgColor rgb="FF696969"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FFFF0000"/>
-        <x:bgColor rgb="FFFF0000"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF0000FF"/>
-        <x:bgColor rgb="FF0000FF"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FFFF1493"/>
-        <x:bgColor rgb="FFFF1493"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FFFFA500"/>
-        <x:bgColor rgb="FFFFA500"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF40E0D0"/>
-        <x:bgColor rgb="FF40E0D0"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF00FFFF"/>
-        <x:bgColor rgb="FF00FFFF"/>
       </x:patternFill>
     </x:fill>
   </x:fills>

</xml_diff>